<commit_message>
Added new benchmark results.
Former-commit-id: 12dd394efed162bffdb05aaf1f443e84c0207ac3
</commit_message>
<xml_diff>
--- a/gidb/tsc_benchmark_results.xlsx
+++ b/gidb/tsc_benchmark_results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="764"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="764" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="9827_2#49" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="49">
   <si>
     <t>Local path</t>
   </si>
@@ -165,10 +165,10 @@
     <t>Intel® Xeon® CPU E5-2690 v2 @ 3.00 GHz, 126GiB RAM, openSUSE 13.1 (Bottle) (x86_64)</t>
   </si>
   <si>
-    <t>Short SAM file containing 100,000 lines; run with original file produced seg fault</t>
+    <t>Timing statistics</t>
   </si>
   <si>
-    <t>Timing statistics</t>
+    <t>The first 100,000 alignments have been used</t>
   </si>
 </sst>
 </file>
@@ -295,7 +295,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1221,11 +1221,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="219"/>
-        <c:axId val="2064689824"/>
-        <c:axId val="2064693632"/>
+        <c:axId val="-60484064"/>
+        <c:axId val="-60483520"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2064689824"/>
+        <c:axId val="-60484064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1243,7 +1243,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2064693632"/>
+        <c:crossAx val="-60483520"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1251,7 +1251,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2064693632"/>
+        <c:axId val="-60483520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1276,7 +1276,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2064689824"/>
+        <c:crossAx val="-60484064"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1666,11 +1666,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="219"/>
-        <c:axId val="2064676224"/>
-        <c:axId val="2064671328"/>
+        <c:axId val="-130465552"/>
+        <c:axId val="-130458480"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2064676224"/>
+        <c:axId val="-130465552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1688,7 +1688,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2064671328"/>
+        <c:crossAx val="-130458480"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1696,7 +1696,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2064671328"/>
+        <c:axId val="-130458480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1721,7 +1721,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2064676224"/>
+        <c:crossAx val="-130465552"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2352,11 +2352,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="219"/>
-        <c:axId val="2064677312"/>
-        <c:axId val="2064684928"/>
+        <c:axId val="-130460656"/>
+        <c:axId val="-130457936"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2064677312"/>
+        <c:axId val="-130460656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2374,7 +2374,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2064684928"/>
+        <c:crossAx val="-130457936"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2382,7 +2382,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2064684928"/>
+        <c:axId val="-130457936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2407,7 +2407,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2064677312"/>
+        <c:crossAx val="-130460656"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3038,11 +3038,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="219"/>
-        <c:axId val="2064694720"/>
-        <c:axId val="2064692544"/>
+        <c:axId val="-60488960"/>
+        <c:axId val="-60486784"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2064694720"/>
+        <c:axId val="-60488960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3060,7 +3060,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2064692544"/>
+        <c:crossAx val="-60486784"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3068,7 +3068,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2064692544"/>
+        <c:axId val="-60486784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3093,7 +3093,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2064694720"/>
+        <c:crossAx val="-60488960"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3772,8 +3772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3818,6 +3818,9 @@
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="6" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
@@ -4297,7 +4300,7 @@
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4342,6 +4345,9 @@
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="6" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
@@ -4821,7 +4827,7 @@
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4866,6 +4872,9 @@
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="6" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
@@ -5344,8 +5353,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5391,7 +5400,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
@@ -5765,7 +5774,7 @@
     </row>
     <row r="21" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>

</xml_diff>